<commit_message>
finalising the cat page
</commit_message>
<xml_diff>
--- a/files/sub/cats/img/linkss.xlsx
+++ b/files/sub/cats/img/linkss.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Henry PC\Documents\001 Github prog Sharing\Cute_animals\files\sub\cats\img\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C749A973-A5E4-4B39-A527-F1CBC63A5360}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9934149E-6ECF-4B2A-A8A1-58C160BDA0CD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="56">
   <si>
     <t>cute_kitty.jpg</t>
   </si>
@@ -199,7 +199,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -211,6 +211,77 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="7"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF92D050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFCC00CC"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFCCFF66"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00CC99"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -237,11 +308,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -249,6 +330,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF00CC99"/>
+      <color rgb="FFCCFF66"/>
+      <color rgb="FFCC00CC"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -525,14 +613,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:BU21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
-      <selection activeCell="AG2" sqref="AG2:AG20"/>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="AE1" sqref="AE1:AE19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
     <row r="1" spans="2:73" x14ac:dyDescent="0.45">
+      <c r="AB1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>10</v>
+      </c>
       <c r="AH1" s="1"/>
+      <c r="AP1" s="4"/>
       <c r="BD1" s="3"/>
       <c r="BR1" t="s">
         <v>37</v>
@@ -542,6 +637,13 @@
       </c>
     </row>
     <row r="2" spans="2:73" x14ac:dyDescent="0.45">
+      <c r="AB2" t="s">
+        <v>17</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>18</v>
+      </c>
+      <c r="AP2" s="5"/>
       <c r="BR2" t="s">
         <v>38</v>
       </c>
@@ -556,6 +658,13 @@
       <c r="E3" s="3" t="s">
         <v>36</v>
       </c>
+      <c r="AB3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>20</v>
+      </c>
+      <c r="AP3" s="6"/>
       <c r="BR3" t="s">
         <v>39</v>
       </c>
@@ -570,6 +679,13 @@
       <c r="E4" t="s">
         <v>1</v>
       </c>
+      <c r="AB4" t="s">
+        <v>21</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>22</v>
+      </c>
+      <c r="AP4" s="7"/>
       <c r="BR4" t="s">
         <v>40</v>
       </c>
@@ -584,6 +700,13 @@
       <c r="E5" t="s">
         <v>3</v>
       </c>
+      <c r="AB5" t="s">
+        <v>15</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>16</v>
+      </c>
+      <c r="AP5" s="8"/>
       <c r="BR5" t="s">
         <v>15</v>
       </c>
@@ -598,6 +721,13 @@
       <c r="E6" t="s">
         <v>5</v>
       </c>
+      <c r="AB6" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>14</v>
+      </c>
+      <c r="AP6" s="9"/>
       <c r="BR6" t="s">
         <v>41</v>
       </c>
@@ -612,6 +742,13 @@
       <c r="E7" t="s">
         <v>7</v>
       </c>
+      <c r="AB7" t="s">
+        <v>11</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP7" s="10"/>
       <c r="BR7" t="s">
         <v>42</v>
       </c>
@@ -626,6 +763,13 @@
       <c r="E8" t="s">
         <v>10</v>
       </c>
+      <c r="AB8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AP8" s="11"/>
       <c r="BR8" t="s">
         <v>43</v>
       </c>
@@ -640,6 +784,13 @@
       <c r="E9" t="s">
         <v>12</v>
       </c>
+      <c r="AB9" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>5</v>
+      </c>
+      <c r="AP9" s="12"/>
       <c r="BR9" t="s">
         <v>44</v>
       </c>
@@ -654,6 +805,13 @@
       <c r="E10" t="s">
         <v>14</v>
       </c>
+      <c r="AB10" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE10" t="s">
+        <v>7</v>
+      </c>
+      <c r="AP10" s="13"/>
       <c r="BR10" t="s">
         <v>45</v>
       </c>
@@ -668,6 +826,12 @@
       <c r="E11" t="s">
         <v>16</v>
       </c>
+      <c r="AB11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>55</v>
+      </c>
       <c r="BR11" t="s">
         <v>54</v>
       </c>
@@ -682,6 +846,12 @@
       <c r="E12" t="s">
         <v>18</v>
       </c>
+      <c r="AB12" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE12" t="s">
+        <v>23</v>
+      </c>
       <c r="BR12" t="s">
         <v>46</v>
       </c>
@@ -696,6 +866,12 @@
       <c r="E13" t="s">
         <v>20</v>
       </c>
+      <c r="AB13" t="s">
+        <v>35</v>
+      </c>
+      <c r="AE13" t="s">
+        <v>34</v>
+      </c>
       <c r="BR13" t="s">
         <v>47</v>
       </c>
@@ -710,6 +886,12 @@
       <c r="E14" t="s">
         <v>22</v>
       </c>
+      <c r="AB14" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>28</v>
+      </c>
       <c r="BR14" t="s">
         <v>48</v>
       </c>
@@ -724,6 +906,12 @@
       <c r="E15" t="s">
         <v>34</v>
       </c>
+      <c r="AB15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE15" t="s">
+        <v>26</v>
+      </c>
       <c r="BR15" t="s">
         <v>49</v>
       </c>
@@ -738,6 +926,12 @@
       <c r="E16" t="s">
         <v>32</v>
       </c>
+      <c r="AB16" t="s">
+        <v>31</v>
+      </c>
+      <c r="AE16" t="s">
+        <v>30</v>
+      </c>
       <c r="BR16" t="s">
         <v>50</v>
       </c>
@@ -752,6 +946,12 @@
       <c r="E17" t="s">
         <v>30</v>
       </c>
+      <c r="AB17" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE17" t="s">
+        <v>32</v>
+      </c>
       <c r="BR17" t="s">
         <v>51</v>
       </c>
@@ -766,6 +966,12 @@
       <c r="E18" t="s">
         <v>28</v>
       </c>
+      <c r="AB18" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE18" t="s">
+        <v>3</v>
+      </c>
       <c r="BD18" s="2"/>
       <c r="BR18" t="s">
         <v>52</v>
@@ -781,6 +987,12 @@
       <c r="E19" t="s">
         <v>26</v>
       </c>
+      <c r="AB19" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE19" t="s">
+        <v>1</v>
+      </c>
       <c r="BR19" t="s">
         <v>53</v>
       </c>
@@ -805,13 +1017,16 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="BU1:BU19">
-    <sortCondition ref="BU1:BU19"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="AP1:AP19">
+    <sortCondition ref="AP1:AP19"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="E20" r:id="rId1" xr:uid="{10FBF420-9691-4E82-8D7C-E4E714A614FE}"/>
     <hyperlink ref="E3" r:id="rId2" xr:uid="{246E8ABC-1FAD-4493-9B2C-DDEA49F2BC23}"/>
+    <hyperlink ref="AE12" r:id="rId3" xr:uid="{8265EF79-61F3-4B7E-AC49-8F1B9B30BEF3}"/>
+    <hyperlink ref="AE8" r:id="rId4" xr:uid="{E708C4A0-CD3B-4A0F-9F1C-C9570034165B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>